<commit_message>
Main script split into 4 subscripts
</commit_message>
<xml_diff>
--- a/data/template/participants_dataset.xlsx
+++ b/data/template/participants_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Thunder/behave/data/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Work/github/behave/data/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F9958C-5C88-C84E-B0DF-EA8CBF87856C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC359038-8F25-9048-9DC0-048F4B673763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="5700" windowWidth="11600" windowHeight="13100" xr2:uid="{18F86FE8-79EB-A14B-B2D7-08912B07C8F4}"/>
+    <workbookView xWindow="22920" yWindow="5700" windowWidth="11600" windowHeight="13100" activeTab="1" xr2:uid="{18F86FE8-79EB-A14B-B2D7-08912B07C8F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>1: intervention; 2: control; 3:waiting</t>
+  </si>
+  <si>
+    <t>Test_template</t>
+  </si>
+  <si>
+    <t>DatasetType</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>CCO</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Karl Koschutnig; Max Mustermann</t>
+  </si>
+  <si>
+    <t>Funding</t>
   </si>
 </sst>
 </file>
@@ -510,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EE173E-B47F-CB4A-9688-91A95D0EB64A}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -618,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DE44F2-DE9B-1840-9667-7216C044FC34}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +666,45 @@
         <v>23</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>